<commit_message>
checking for already existing strings
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>key</t>
   </si>
@@ -22,22 +22,43 @@
     <t>ID</t>
   </si>
   <si>
+    <t>PH</t>
+  </si>
+  <si>
     <t>app_title</t>
   </si>
   <si>
+    <t>nameNewV2</t>
+  </si>
+  <si>
+    <t>somenameinid</t>
+  </si>
+  <si>
+    <t>namePH</t>
+  </si>
+  <si>
+    <t>next_key</t>
+  </si>
+  <si>
+    <t>NextNewV2</t>
+  </si>
+  <si>
+    <t>Nextinid</t>
+  </si>
+  <si>
+    <t>nextPH</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
-    <t>somenameinid</t>
-  </si>
-  <si>
-    <t>next_key</t>
-  </si>
-  <si>
-    <t>next</t>
-  </si>
-  <si>
-    <t>Nextinid</t>
+    <t>engName</t>
+  </si>
+  <si>
+    <t>IdName</t>
+  </si>
+  <si>
+    <t>phName</t>
   </si>
 </sst>
 </file>
@@ -176,13 +197,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1301,76 +1322,90 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
+      <c r="A4" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="6"/>

</xml_diff>